<commit_message>
Updated Black Desert commands so they actually function now
</commit_message>
<xml_diff>
--- a/cogs/memberGearSheets.xlsx
+++ b/cogs/memberGearSheets.xlsx
@@ -440,21 +440,25 @@
           <t>Mystic</t>
         </is>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>190</v>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>198</t>
+        </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>183</t>
+          <t>208</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>486</v>
+          <t>298</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>501</t>
+        </is>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="3" s="2"/>

</xml_diff>